<commit_message>
Added bathyergidae date. Corrected name of Xenarthran element
</commit_message>
<xml_diff>
--- a/tabular/locus-side-data.xlsx
+++ b/tabular/locus-side-data.xlsx
@@ -1,22 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/Ortervirales/HIV-GLUE/tabular/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{796F9004-4509-0146-84E7-E64CE2D7B991}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="24030"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="15080" yWindow="1340" windowWidth="27640" windowHeight="16940" xr2:uid="{2FAEDAF0-1D48-DD48-BB7A-BD985ADBB976}"/>
+    <workbookView xWindow="15080" yWindow="1340" windowWidth="27640" windowHeight="16940"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -31,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="57">
   <si>
     <t>Bathyergidae</t>
   </si>
@@ -108,12 +105,6 @@
     <t>EFLN.Filo.31-Soricidae</t>
   </si>
   <si>
-    <t xml:space="preserve">Xenarthra </t>
-  </si>
-  <si>
-    <t>EFLN.Filo.41-Xenarthra</t>
-  </si>
-  <si>
     <t>Monodelphis</t>
   </si>
   <si>
@@ -192,22 +183,35 @@
     <t>Number-dupes</t>
   </si>
   <si>
-    <t>Ortho-age</t>
-  </si>
-  <si>
     <t>Clock-age</t>
+  </si>
+  <si>
+    <t>Ortho-age (MYA)</t>
+  </si>
+  <si>
+    <t>Ortho-age CI (MYA)</t>
+  </si>
+  <si>
+    <t>28-40</t>
+  </si>
+  <si>
+    <t>Vermilingua</t>
+  </si>
+  <si>
+    <t>EFLN.Filo.41-Vermilingua</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -224,6 +228,24 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -268,18 +290,43 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="9">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -343,7 +390,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -395,7 +442,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -589,47 +636,52 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D2D0A86-A3BA-D343-B405-6F8A8A5D100C}">
-  <dimension ref="A1:F26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F26" sqref="A1:F26"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="25.1640625" customWidth="1"/>
     <col min="2" max="2" width="21.6640625" customWidth="1"/>
+    <col min="5" max="5" width="18.5" style="8" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -642,10 +694,15 @@
       <c r="D2" s="3">
         <v>2</v>
       </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E2" s="7">
+        <v>34</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="G2" s="3"/>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -658,10 +715,11 @@
       <c r="D3" s="3">
         <v>1</v>
       </c>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="3"/>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
@@ -674,10 +732,11 @@
       <c r="D4" s="3">
         <v>1</v>
       </c>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="3"/>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -690,10 +749,11 @@
       <c r="D5" s="3">
         <v>3</v>
       </c>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="3"/>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -706,10 +766,11 @@
       <c r="D6" s="3">
         <v>5</v>
       </c>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="3"/>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
@@ -722,10 +783,11 @@
       <c r="D7" s="3">
         <v>1</v>
       </c>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="3"/>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
@@ -738,10 +800,11 @@
       <c r="D8" s="3">
         <v>2</v>
       </c>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="3"/>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" s="2" t="s">
         <v>15</v>
       </c>
@@ -754,10 +817,11 @@
       <c r="D9" s="3">
         <v>2</v>
       </c>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="3"/>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10" s="2" t="s">
         <v>17</v>
       </c>
@@ -770,10 +834,11 @@
       <c r="D10" s="3">
         <v>5</v>
       </c>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="3"/>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11" s="2" t="s">
         <v>19</v>
       </c>
@@ -786,10 +851,11 @@
       <c r="D11" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="3"/>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12" s="2" t="s">
         <v>22</v>
       </c>
@@ -802,10 +868,11 @@
       <c r="D12" s="3">
         <v>3</v>
       </c>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="3"/>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13" s="2" t="s">
         <v>24</v>
       </c>
@@ -818,15 +885,16 @@
       <c r="D13" s="3">
         <v>2</v>
       </c>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="3"/>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14" s="2" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="C14" s="3">
         <v>2</v>
@@ -834,31 +902,33 @@
       <c r="D14" s="3">
         <v>1</v>
       </c>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="3"/>
+    </row>
+    <row r="15" spans="1:7">
       <c r="A15" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="3">
+        <v>1</v>
+      </c>
+      <c r="D15" s="3">
+        <v>1</v>
+      </c>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="3"/>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B16" s="5" t="s">
         <v>27</v>
-      </c>
-      <c r="C15" s="3">
-        <v>1</v>
-      </c>
-      <c r="D15" s="3">
-        <v>1</v>
-      </c>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>29</v>
       </c>
       <c r="C16" s="3">
         <v>3</v>
@@ -866,28 +936,30 @@
       <c r="D16" s="3">
         <v>13</v>
       </c>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="3"/>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B17" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="3">
+        <v>1</v>
+      </c>
+      <c r="D17" s="3">
+        <v>1</v>
+      </c>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="3"/>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="C17" s="3">
-        <v>1</v>
-      </c>
-      <c r="D17" s="3">
-        <v>1</v>
-      </c>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
-        <v>33</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>6</v>
@@ -898,31 +970,33 @@
       <c r="D18" s="3">
         <v>7</v>
       </c>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="3"/>
+    </row>
+    <row r="19" spans="1:7">
       <c r="A19" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="3">
+        <v>1</v>
+      </c>
+      <c r="D19" s="3">
+        <v>1</v>
+      </c>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="3"/>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B20" s="5" t="s">
         <v>34</v>
-      </c>
-      <c r="C19" s="3">
-        <v>1</v>
-      </c>
-      <c r="D19" s="3">
-        <v>1</v>
-      </c>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>36</v>
       </c>
       <c r="C20" s="3">
         <v>9</v>
@@ -930,47 +1004,50 @@
       <c r="D20" s="3">
         <v>3</v>
       </c>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="3"/>
+    </row>
+    <row r="21" spans="1:7">
       <c r="A21" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" s="3">
+        <v>1</v>
+      </c>
+      <c r="D21" s="3">
+        <v>1</v>
+      </c>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="3"/>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B22" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C21" s="3">
-        <v>1</v>
-      </c>
-      <c r="D21" s="3">
-        <v>1</v>
-      </c>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
+      <c r="C22" s="3">
+        <v>1</v>
+      </c>
+      <c r="D22" s="3">
+        <v>1</v>
+      </c>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="3"/>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B23" s="5" t="s">
         <v>40</v>
-      </c>
-      <c r="C22" s="3">
-        <v>1</v>
-      </c>
-      <c r="D22" s="3">
-        <v>1</v>
-      </c>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>42</v>
       </c>
       <c r="C23" s="3">
         <v>4</v>
@@ -978,15 +1055,16 @@
       <c r="D23" s="3">
         <v>1</v>
       </c>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="3"/>
+    </row>
+    <row r="24" spans="1:7">
       <c r="A24" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C24" s="3">
         <v>1</v>
@@ -994,15 +1072,16 @@
       <c r="D24" s="3">
         <v>2</v>
       </c>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="3"/>
+    </row>
+    <row r="25" spans="1:7">
       <c r="A25" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C25" s="3">
         <v>1</v>
@@ -1010,12 +1089,13 @@
       <c r="D25" s="3">
         <v>4</v>
       </c>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="3"/>
+    </row>
+    <row r="26" spans="1:7">
       <c r="A26" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>6</v>
@@ -1026,10 +1106,17 @@
       <c r="D26" s="3">
         <v>1</v>
       </c>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added TimeTree dates for orthologous inserts
</commit_message>
<xml_diff>
--- a/tabular/locus-side-data.xlsx
+++ b/tabular/locus-side-data.xlsx
@@ -1,34 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="24030"/>
-  <workbookPr autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/virus/comparative/Filoviridae-EVE/tabular/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EA4A7B0-C055-F945-B12A-CF8D9CEF6C36}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15080" yWindow="1340" windowWidth="27640" windowHeight="16940"/>
+    <workbookView xWindow="8300" yWindow="460" windowWidth="20540" windowHeight="14440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="66">
   <si>
     <t>Bathyergidae</t>
   </si>
@@ -42,9 +42,6 @@
     <t>EFLN.Filo.2-Caviomorpha</t>
   </si>
   <si>
-    <t>Dipodidae</t>
-  </si>
-  <si>
     <t>EFLN.Filo.3-Dipodidae</t>
   </si>
   <si>
@@ -54,9 +51,6 @@
     <t>EFLN.Filo.4-Cricetidae</t>
   </si>
   <si>
-    <t>Mus</t>
-  </si>
-  <si>
     <t>EFLN.Filo.5-Mus</t>
   </si>
   <si>
@@ -78,9 +72,6 @@
     <t>EFLN.Filo.8-Dipodomys</t>
   </si>
   <si>
-    <t>Spalacidae</t>
-  </si>
-  <si>
     <t>EFLN.Filo.9-Spalacidae</t>
   </si>
   <si>
@@ -90,12 +81,6 @@
     <t>EFLN.Filo.10-Neotominae</t>
   </si>
   <si>
-    <t>5?</t>
-  </si>
-  <si>
-    <t>Vespertilionidae</t>
-  </si>
-  <si>
     <t>EFLN.Filo.21-Vespertilionidae</t>
   </si>
   <si>
@@ -111,9 +96,6 @@
     <t>EFLN.Filo.51-Monodelphis</t>
   </si>
   <si>
-    <t>Diprotodontia</t>
-  </si>
-  <si>
     <t>EFLN.Filo.61-Diprotodontia</t>
   </si>
   <si>
@@ -195,16 +177,61 @@
     <t>28-40</t>
   </si>
   <si>
-    <t>Vermilingua</t>
-  </si>
-  <si>
-    <t>EFLN.Filo.41-Vermilingua</t>
+    <t>23.1-34.0</t>
+  </si>
+  <si>
+    <t>18-48</t>
+  </si>
+  <si>
+    <t>Dipodidae (descendant unranked)</t>
+  </si>
+  <si>
+    <t>28-39</t>
+  </si>
+  <si>
+    <t>NK</t>
+  </si>
+  <si>
+    <t>Mus (descendant unranked)</t>
+  </si>
+  <si>
+    <t>6-10.6</t>
+  </si>
+  <si>
+    <t>10.8-32.8</t>
+  </si>
+  <si>
+    <t>Spalacidae (descendant unranked)</t>
+  </si>
+  <si>
+    <t>22-44</t>
+  </si>
+  <si>
+    <t>Vespertilionidae (descendant unranked)</t>
+  </si>
+  <si>
+    <t>27-36</t>
+  </si>
+  <si>
+    <t>Myrmecophagidae</t>
+  </si>
+  <si>
+    <t>EFLN.Filo.41-Myrmecophagidae</t>
+  </si>
+  <si>
+    <t>31-40</t>
+  </si>
+  <si>
+    <t>Diprotodontia (descendant unranked)</t>
+  </si>
+  <si>
+    <t>10.1-16</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -249,7 +276,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -280,6 +307,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -301,7 +334,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -315,6 +348,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -636,52 +672,54 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="25.1640625" customWidth="1"/>
-    <col min="2" max="2" width="21.6640625" customWidth="1"/>
+    <col min="2" max="2" width="34.6640625" customWidth="1"/>
+    <col min="3" max="3" width="15.1640625" customWidth="1"/>
     <col min="5" max="5" width="18.5" style="8" customWidth="1"/>
-    <col min="6" max="6" width="10.83203125" style="8" customWidth="1"/>
+    <col min="6" max="6" width="25.83203125" style="8" customWidth="1"/>
+    <col min="7" max="7" width="21.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="F1" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>53</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -698,11 +736,11 @@
         <v>34</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="G2" s="3"/>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -715,16 +753,20 @@
       <c r="D3" s="3">
         <v>1</v>
       </c>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
+      <c r="E3" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>53</v>
+      </c>
       <c r="G3" s="3"/>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>4</v>
+        <v>51</v>
       </c>
       <c r="C4" s="3">
         <v>2</v>
@@ -732,16 +774,20 @@
       <c r="D4" s="3">
         <v>1</v>
       </c>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
+      <c r="E4" s="7">
+        <v>34</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>52</v>
+      </c>
       <c r="G4" s="3"/>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5" s="3">
         <v>10</v>
@@ -749,16 +795,20 @@
       <c r="D5" s="3">
         <v>3</v>
       </c>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
+      <c r="E5" s="7">
+        <v>31</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>50</v>
+      </c>
       <c r="G5" s="3"/>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>8</v>
+        <v>54</v>
       </c>
       <c r="C6" s="3">
         <v>8</v>
@@ -766,33 +816,41 @@
       <c r="D6" s="3">
         <v>5</v>
       </c>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
+      <c r="E6" s="7">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>55</v>
+      </c>
       <c r="G6" s="3"/>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="3">
+        <v>1</v>
+      </c>
+      <c r="D7" s="3">
+        <v>1</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="G7" s="3"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B8" s="5" t="s">
         <v>10</v>
-      </c>
-      <c r="C7" s="3">
-        <v>1</v>
-      </c>
-      <c r="D7" s="3">
-        <v>1</v>
-      </c>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="3"/>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>12</v>
       </c>
       <c r="C8" s="3">
         <v>1</v>
@@ -800,16 +858,20 @@
       <c r="D8" s="3">
         <v>2</v>
       </c>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
+      <c r="E8" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>53</v>
+      </c>
       <c r="G8" s="3"/>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C9" s="3">
         <v>1</v>
@@ -817,16 +879,20 @@
       <c r="D9" s="3">
         <v>2</v>
       </c>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
+      <c r="E9" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>53</v>
+      </c>
       <c r="G9" s="3"/>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>16</v>
+        <v>57</v>
       </c>
       <c r="C10" s="3">
         <v>2</v>
@@ -834,33 +900,41 @@
       <c r="D10" s="3">
         <v>5</v>
       </c>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
+      <c r="E10" s="7">
+        <v>33</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>58</v>
+      </c>
       <c r="G10" s="3"/>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C11" s="3">
-        <v>4</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
+        <v>1</v>
+      </c>
+      <c r="D11" s="3">
+        <v>5</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>53</v>
+      </c>
       <c r="G11" s="3"/>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>21</v>
+        <v>59</v>
       </c>
       <c r="C12" s="3">
         <v>7</v>
@@ -868,16 +942,20 @@
       <c r="D12" s="3">
         <v>3</v>
       </c>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
+      <c r="E12" s="7">
+        <v>31</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="G12" s="3"/>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C13" s="3">
         <v>1</v>
@@ -885,16 +963,20 @@
       <c r="D13" s="3">
         <v>2</v>
       </c>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
+      <c r="E13" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>53</v>
+      </c>
       <c r="G13" s="3"/>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="C14" s="3">
         <v>2</v>
@@ -902,16 +984,20 @@
       <c r="D14" s="3">
         <v>1</v>
       </c>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
+      <c r="E14" s="7">
+        <v>13.1</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>65</v>
+      </c>
       <c r="G14" s="3"/>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C15" s="3">
         <v>1</v>
@@ -919,16 +1005,20 @@
       <c r="D15" s="3">
         <v>1</v>
       </c>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
+      <c r="E15" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>53</v>
+      </c>
       <c r="G15" s="3"/>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>27</v>
+        <v>64</v>
       </c>
       <c r="C16" s="3">
         <v>3</v>
@@ -936,16 +1026,20 @@
       <c r="D16" s="3">
         <v>13</v>
       </c>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
+      <c r="E16" s="7">
+        <v>35</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>63</v>
+      </c>
       <c r="G16" s="3"/>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C17" s="3">
         <v>1</v>
@@ -953,16 +1047,20 @@
       <c r="D17" s="3">
         <v>1</v>
       </c>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
+      <c r="E17" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>53</v>
+      </c>
       <c r="G17" s="3"/>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C18" s="3">
         <v>11</v>
@@ -970,16 +1068,20 @@
       <c r="D18" s="3">
         <v>7</v>
       </c>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
+      <c r="E18" s="7">
+        <v>31</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>50</v>
+      </c>
       <c r="G18" s="3"/>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C19" s="3">
         <v>1</v>
@@ -987,16 +1089,20 @@
       <c r="D19" s="3">
         <v>1</v>
       </c>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
+      <c r="E19" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>53</v>
+      </c>
       <c r="G19" s="3"/>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C20" s="3">
         <v>9</v>
@@ -1004,16 +1110,20 @@
       <c r="D20" s="3">
         <v>3</v>
       </c>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
+      <c r="E20" s="7">
+        <v>28.6</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>49</v>
+      </c>
       <c r="G20" s="3"/>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C21" s="3">
         <v>1</v>
@@ -1021,16 +1131,20 @@
       <c r="D21" s="3">
         <v>1</v>
       </c>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
+      <c r="E21" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="F21" s="9" t="s">
+        <v>53</v>
+      </c>
       <c r="G21" s="3"/>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C22" s="3">
         <v>1</v>
@@ -1038,16 +1152,20 @@
       <c r="D22" s="3">
         <v>1</v>
       </c>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
+      <c r="E22" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>53</v>
+      </c>
       <c r="G22" s="3"/>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C23" s="3">
         <v>4</v>
@@ -1055,16 +1173,20 @@
       <c r="D23" s="3">
         <v>1</v>
       </c>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
+      <c r="E23" s="7">
+        <v>20.8</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>56</v>
+      </c>
       <c r="G23" s="3"/>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C24" s="3">
         <v>1</v>
@@ -1072,16 +1194,20 @@
       <c r="D24" s="3">
         <v>2</v>
       </c>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
+      <c r="E24" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>53</v>
+      </c>
       <c r="G24" s="3"/>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C25" s="3">
         <v>1</v>
@@ -1089,16 +1215,20 @@
       <c r="D25" s="3">
         <v>4</v>
       </c>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
+      <c r="E25" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="F25" s="9" t="s">
+        <v>53</v>
+      </c>
       <c r="G25" s="3"/>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C26" s="3">
         <v>5</v>
@@ -1106,8 +1236,12 @@
       <c r="D26" s="3">
         <v>1</v>
       </c>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
+      <c r="E26" s="7">
+        <v>31</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>50</v>
+      </c>
       <c r="G26" s="3"/>
     </row>
   </sheetData>

</xml_diff>